<commit_message>
Cleaned up bugs and fixed the log lifts class, which was not working after adding in the export to excel functionality. Was mostly just an issue of fixing the SQL syntax. Next up, allow user to change the date of each entry.
</commit_message>
<xml_diff>
--- a/fitness_data.xlsx
+++ b/fitness_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14280" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14200" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="diet" sheetId="1" state="visible" r:id="rId1"/>
@@ -419,8 +419,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -456,40 +456,26 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>44201</v>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>2222</v>
+        <v>2000</v>
       </c>
       <c r="C2" t="n">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
-        <v>432</v>
+        <v>43</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1233</v>
-      </c>
-      <c r="C3" t="n">
-        <v>123</v>
-      </c>
-      <c r="D3" t="n">
-        <v>123</v>
-      </c>
-      <c r="E3" t="n">
-        <v>123</v>
-      </c>
+      <c r="A3" s="4" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="n"/>
@@ -505,10 +491,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -545,119 +531,25 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>44201</v>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>236</v>
+        <v>12.3</v>
       </c>
       <c r="C2" t="n">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>12.3</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>323.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>323.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>87.6</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>554.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>88.8</v>
-      </c>
-      <c r="C6" t="n">
-        <v>888.8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1232</v>
-      </c>
-      <c r="C7" t="n">
-        <v>123</v>
-      </c>
-      <c r="D7" t="n">
-        <v>123</v>
-      </c>
-      <c r="E7" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>111.1</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>y</t>
+        <v>234.3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>n</t>
         </is>
       </c>
     </row>
@@ -676,7 +568,7 @@
   <dimension ref="A1:F224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -716,7 +608,7 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -730,21 +622,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -758,21 +648,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -786,21 +674,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F4" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -814,21 +700,19 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F5" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -842,21 +726,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E6" t="n">
         <v>3</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F6" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -870,21 +752,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F7" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -898,21 +778,19 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F8" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -926,21 +804,19 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F9" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -959,16 +835,14 @@
       <c r="E10" t="n">
         <v>1</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F10" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -987,16 +861,14 @@
       <c r="E11" t="n">
         <v>2</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F11" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1015,16 +887,14 @@
       <c r="E12" t="n">
         <v>3</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F12" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1043,16 +913,14 @@
       <c r="E13" t="n">
         <v>1</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F13" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1071,16 +939,14 @@
       <c r="E14" t="n">
         <v>2</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F14" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1099,16 +965,14 @@
       <c r="E15" t="n">
         <v>3</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F15" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1127,16 +991,14 @@
       <c r="E16" t="n">
         <v>4</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F16" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1149,24 +1011,20 @@
           <t>Hammer_Curl</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>213</t>
-        </is>
+      <c r="D17" t="n">
+        <v>15</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F17" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1179,24 +1037,20 @@
           <t>Hammer_Curl</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>213</t>
-        </is>
+      <c r="D18" t="n">
+        <v>15</v>
       </c>
       <c r="E18" t="n">
         <v>2</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F18" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1209,24 +1063,20 @@
           <t>Hammer_Curl</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>213</t>
-        </is>
+      <c r="D19" t="n">
+        <v>15</v>
       </c>
       <c r="E19" t="n">
         <v>3</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F19" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>2021-01-06</t>
+          <t>2021-01-09</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1239,76 +1089,509 @@
           <t>Hammer_Curl</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>213</t>
-        </is>
+      <c r="D20" t="n">
+        <v>15</v>
       </c>
       <c r="E20" t="n">
         <v>4</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F20" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n"/>
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Deadlift</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>115</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n"/>
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Deadlift</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>115</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n"/>
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Lat_Pulldown</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>88</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n"/>
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Lat_Pulldown</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>88</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n"/>
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Lat_Pulldown</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>88</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n"/>
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Cable_Row</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>88</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n"/>
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Cable_Row</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>88</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n"/>
+      <c r="A28" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Cable_Row</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>88</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n"/>
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Rear_Delt_Lateral_Raise</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>15</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n"/>
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Rear_Delt_Lateral_Raise</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>15</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n"/>
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Rear_Delt_Lateral_Raise</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>15</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n"/>
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Preacher_Curls</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>30</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n"/>
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Preacher_Curls</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>30</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n"/>
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Preacher_Curls</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>30</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="n"/>
+      <c r="A35" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Preacher_Curls</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>30</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4</v>
+      </c>
+      <c r="F35" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="n"/>
+      <c r="A36" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hammer_Curl</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>15</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n"/>
+      <c r="A37" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hammer_Curl</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>15</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="n"/>
+      <c r="A38" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hammer_Curl</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>15</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3</v>
+      </c>
+      <c r="F38" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="n"/>
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Pull_1</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hammer_Curl</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>15</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4</v>
+      </c>
+      <c r="F39" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="n"/>
@@ -1877,10 +2160,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1906,28 +2189,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>44201</v>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-09</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>26.3</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.03162037037037037</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>12:12:12</t>
+        <v>26.2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>04:43:12</t>
         </is>
       </c>
     </row>

</xml_diff>